<commit_message>
MOSIP-11739_added template for additional info email subject (#640)
* MOSIP-15883

* MOSIP-15883

* Update master-template.csv

* Update master-template.csv

* Update master-template.csv

* Update master-template_type.csv

* MOSIP-11739

* Update master-template.csv

* Update master-template_type.csv

* Add files via upload

* Add files via upload
</commit_message>
<xml_diff>
--- a/data-dml/mosip_master/dml/master-template_type.xlsx
+++ b/data-dml/mosip_master/dml/master-template_type.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="296">
   <si>
     <t>code</t>
   </si>
@@ -902,6 +902,12 @@
   </si>
   <si>
     <t>Registration Failed because you have already Registered</t>
+  </si>
+  <si>
+    <t>RPR_PAUSED_FOR_ADDITIONAL_INFO_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>Requesting the additional details for progressing on the application of UIN</t>
   </si>
 </sst>
 </file>
@@ -1745,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F146" sqref="F146"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4677,6 +4683,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>294</v>
+      </c>
+      <c r="B147" t="s">
+        <v>295</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" t="b">
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>